<commit_message>
bastante completo, falta arreglar unos bugs
</commit_message>
<xml_diff>
--- a/perfiles.xlsx
+++ b/perfiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matias\Desktop\scrap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45B5F8A-0712-4C61-9C4B-80AEA0B3AEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13D4515-91AE-4B40-91A7-E7F6FF0E1AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -803,7 +803,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>